<commit_message>
update tag based cf
</commit_message>
<xml_diff>
--- a/docs/matlab/hetrec2011delicious2k.xlsx
+++ b/docs/matlab/hetrec2011delicious2k.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="UserKNN" sheetId="1" r:id="rId1"/>
+    <sheet name="TagBasedFiltering" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="15">
   <si>
     <t>K(Cosine)</t>
   </si>
@@ -41,12 +42,36 @@
     <t>9 vs 1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>train</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>userTags</t>
+  </si>
+  <si>
+    <t>itemTags</t>
+  </si>
+  <si>
+    <t>Simple</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TFIDF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TFIDF++</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,13 +92,26 @@
       <name val="Calibri Light"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -85,16 +123,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="58" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="好" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -107,6 +150,1265 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.15576139540602232"/>
+          <c:y val="3.6712552539420663E-2"/>
+          <c:w val="0.79286025092077339"/>
+          <c:h val="0.81243801307566044"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TagBasedFiltering!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Simple</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>TagBasedFiltering!$B$6:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>5.93311758360302E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.6776636019469999E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.9810298102980999E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.60529743812419E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.1186440677966102E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.82644430432041E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.6133710390834599E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>TagBasedFiltering!$C$6:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.0366600697389501E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.2042220337385702E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.1833003486947502E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.7854113655640398E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.3508623126943701E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.9163132598247098E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.3875223824333208E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TagBasedFiltering!$C$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>TFIDF</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>TagBasedFiltering!$B$19:$B$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>4.8622366288492702E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.4434810881109803E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.5842293906810001E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.1182015953589602E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.6949041811846698E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.4405656882613099E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.3799574877822801E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>TagBasedFiltering!$C$19:$C$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>8.60749808722265E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.9211935730680903E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.3121652639632703E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.22494261667942E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.4682478959449094E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.07115531752104E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.25286916602907E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TagBasedFiltering!$C$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>TFIDF++</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>TagBasedFiltering!$B$32:$B$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>7.5431034482758598E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.3210543372582903E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.30229536595929E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.8548713501011899E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.49606598296164E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.3893305530214202E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.1733618285217499E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>TagBasedFiltering!$C$32:$C$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.33181126331811E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.8051750380517502E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.8028919330289199E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.5152207001522101E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.7519025875190306E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0464231354642301E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1415525114155301E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="328956208"/>
+        <c:axId val="328952944"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="328956208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>P@N</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-CN"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="328952944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="328952944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>R@N</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-CN"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="328956208"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.77823457403873397"/>
+          <c:y val="5.6528658654202438E-2"/>
+          <c:w val="0.20877164285217911"/>
+          <c:h val="0.19181060422501825"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1200">
+          <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>590549</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>466724</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="图表 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -398,7 +1700,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1178,4 +2480,541 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="12.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1">
+        <v>94188</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1">
+        <v>10611</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1">
+        <v>214336</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1">
+        <v>370737</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1">
+        <v>5.93311758360302E-3</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1.0366600697389501E-3</v>
+      </c>
+      <c r="D6" s="1">
+        <v>4.9334450339756104E-3</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2.6232614897798801</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3.6776636019469999E-3</v>
+      </c>
+      <c r="C7" s="1">
+        <v>3.2042220337385702E-3</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2.06335908653697E-2</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2.4336530029561798</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2.9810298102980999E-3</v>
+      </c>
+      <c r="C8" s="1">
+        <v>5.1833003486947502E-3</v>
+      </c>
+      <c r="D8" s="1">
+        <v>3.8940085016599998E-2</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2.31977602474513</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2.60529743812419E-3</v>
+      </c>
+      <c r="C9" s="1">
+        <v>6.7854113655640398E-3</v>
+      </c>
+      <c r="D9" s="1">
+        <v>5.6579478109776898E-2</v>
+      </c>
+      <c r="E9" s="1">
+        <v>2.2456570655117898</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1">
+        <v>2.1186440677966102E-3</v>
+      </c>
+      <c r="C10" s="1">
+        <v>7.3508623126943701E-3</v>
+      </c>
+      <c r="D10" s="1">
+        <v>7.3179434670638199E-2</v>
+      </c>
+      <c r="E10" s="1">
+        <v>2.1903669873012199</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>25</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1.82644430432041E-3</v>
+      </c>
+      <c r="C11" s="1">
+        <v>7.9163132598247098E-3</v>
+      </c>
+      <c r="D11" s="1">
+        <v>9.0524062180024206E-2</v>
+      </c>
+      <c r="E11" s="1">
+        <v>2.1441612715417899</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>30</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1.6133710390834599E-3</v>
+      </c>
+      <c r="C12" s="1">
+        <v>8.3875223824333208E-3</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.10766700797418501</v>
+      </c>
+      <c r="E12" s="1">
+        <v>2.1057715073424701</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="1">
+        <v>94343</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="1">
+        <v>10456</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="1">
+        <v>214115</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="1">
+        <v>371147</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>1</v>
+      </c>
+      <c r="B19" s="1">
+        <v>4.8622366288492702E-3</v>
+      </c>
+      <c r="C19" s="1">
+        <v>8.60749808722265E-4</v>
+      </c>
+      <c r="D19" s="1">
+        <v>7.4134962854971497E-3</v>
+      </c>
+      <c r="E19" s="1">
+        <v>2.47052137310834</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>5</v>
+      </c>
+      <c r="B20" s="1">
+        <v>4.4434810881109803E-3</v>
+      </c>
+      <c r="C20" s="1">
+        <v>3.9211935730680903E-3</v>
+      </c>
+      <c r="D20" s="1">
+        <v>3.0491493090559402E-2</v>
+      </c>
+      <c r="E20" s="1">
+        <v>2.3010801998357602</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>10</v>
+      </c>
+      <c r="B21" s="1">
+        <v>3.5842293906810001E-3</v>
+      </c>
+      <c r="C21" s="1">
+        <v>6.3121652639632703E-3</v>
+      </c>
+      <c r="D21" s="1">
+        <v>5.6997068722180001E-2</v>
+      </c>
+      <c r="E21" s="1">
+        <v>2.2046928206640799</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>15</v>
+      </c>
+      <c r="B22" s="1">
+        <v>3.1182015953589602E-3</v>
+      </c>
+      <c r="C22" s="1">
+        <v>8.22494261667942E-3</v>
+      </c>
+      <c r="D22" s="1">
+        <v>8.1501930921103694E-2</v>
+      </c>
+      <c r="E22" s="1">
+        <v>2.1345353259593498</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>20</v>
+      </c>
+      <c r="B23" s="1">
+        <v>2.6949041811846698E-3</v>
+      </c>
+      <c r="C23" s="1">
+        <v>9.4682478959449094E-3</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0.104471361880981</v>
+      </c>
+      <c r="E23" s="1">
+        <v>2.0871292336620102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>25</v>
+      </c>
+      <c r="B24" s="1">
+        <v>2.4405656882613099E-3</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1.07115531752104E-2</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0.12567272050498601</v>
+      </c>
+      <c r="E24" s="1">
+        <v>2.0469024182736399</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>30</v>
+      </c>
+      <c r="B25" s="1">
+        <v>2.3799574877822801E-3</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1.25286916602907E-2</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0.14597453355460099</v>
+      </c>
+      <c r="E25" s="1">
+        <v>2.0124780450917599</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="1">
+        <v>94287</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="1">
+        <v>10512</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="1">
+        <v>214565</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" s="1">
+        <v>371655</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>1</v>
+      </c>
+      <c r="B32" s="1">
+        <v>7.5431034482758598E-3</v>
+      </c>
+      <c r="C32" s="1">
+        <v>1.33181126331811E-3</v>
+      </c>
+      <c r="D32" s="1">
+        <v>1.16109629813356E-2</v>
+      </c>
+      <c r="E32" s="1">
+        <v>2.0261921256038198</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>5</v>
+      </c>
+      <c r="B33" s="1">
+        <v>4.3210543372582903E-3</v>
+      </c>
+      <c r="C33" s="1">
+        <v>3.8051750380517502E-3</v>
+      </c>
+      <c r="D33" s="1">
+        <v>5.11409437589136E-2</v>
+      </c>
+      <c r="E33" s="1">
+        <v>1.86242544695432</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>10</v>
+      </c>
+      <c r="B34" s="1">
+        <v>3.30229536595929E-3</v>
+      </c>
+      <c r="C34" s="1">
+        <v>5.8028919330289199E-3</v>
+      </c>
+      <c r="D34" s="1">
+        <v>9.53835183233087E-2</v>
+      </c>
+      <c r="E34" s="1">
+        <v>1.76067950528269</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>15</v>
+      </c>
+      <c r="B35" s="1">
+        <v>2.8548713501011899E-3</v>
+      </c>
+      <c r="C35" s="1">
+        <v>7.5152207001522101E-3</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0.13593662801513001</v>
+      </c>
+      <c r="E35" s="1">
+        <v>1.70135039416123</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>20</v>
+      </c>
+      <c r="B36" s="1">
+        <v>2.49606598296164E-3</v>
+      </c>
+      <c r="C36" s="1">
+        <v>8.7519025875190306E-3</v>
+      </c>
+      <c r="D36" s="1">
+        <v>0.172459229862963</v>
+      </c>
+      <c r="E36" s="1">
+        <v>1.66297705580509</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>25</v>
+      </c>
+      <c r="B37" s="1">
+        <v>2.3893305530214202E-3</v>
+      </c>
+      <c r="C37" s="1">
+        <v>1.0464231354642301E-2</v>
+      </c>
+      <c r="D37" s="1">
+        <v>0.206842562162833</v>
+      </c>
+      <c r="E37" s="1">
+        <v>1.6316452379600499</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>30</v>
+      </c>
+      <c r="B38" s="1">
+        <v>2.1733618285217499E-3</v>
+      </c>
+      <c r="C38" s="1">
+        <v>1.1415525114155301E-2</v>
+      </c>
+      <c r="D38" s="1">
+        <v>0.240342283127674</v>
+      </c>
+      <c r="E38" s="1">
+        <v>1.6024482389478301</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>